<commit_message>
Cross referneced ~99% of the ReGrid API with qPublic scraping, and added DRAFT Hugging Face Datasets to store this info in
</commit_message>
<xml_diff>
--- a/DatasetConfiguration/DatasetDocumentation.xlsx
+++ b/DatasetConfiguration/DatasetDocumentation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>BuildingInfoTable</t>
   </si>
@@ -74,7 +74,7 @@
     <t>effectiveYearBuilt</t>
   </si>
   <si>
-    <t>SQlite</t>
+    <t>SeleniumSoupQPublic.py</t>
   </si>
   <si>
     <t>OpenSearch Database</t>
@@ -83,9 +83,21 @@
     <t>Hugging Face Dataset #</t>
   </si>
   <si>
+    <t>1,2</t>
+  </si>
+  <si>
     <t>ReGrid API</t>
   </si>
   <si>
+    <t>DATA NOT AVAILABLE</t>
+  </si>
+  <si>
+    <t>recrdareano</t>
+  </si>
+  <si>
+    <t>yearbuilt</t>
+  </si>
+  <si>
     <t>ExtraFeaturesTable</t>
   </si>
   <si>
@@ -125,6 +137,30 @@
     <t>postalCode</t>
   </si>
   <si>
+    <t>owner_name = owner_element.find("span", {"id": "ctlBodyPane_ctl01_ctl01_rptOwner_ctl00_sprOwnerName1_lnkUpmSearchLinkSuppressed_lblSearch"}).text</t>
+  </si>
+  <si>
+    <t>parse_raw_owner_address(owner_name, owner_address)</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>mailadd</t>
+  </si>
+  <si>
+    <t>mail_city</t>
+  </si>
+  <si>
+    <t>mail_state2</t>
+  </si>
+  <si>
+    <t>mail_zip</t>
+  </si>
+  <si>
     <t>ParcelSummaryTable</t>
   </si>
   <si>
@@ -149,12 +185,54 @@
     <t>gpsPolygonCoordinates</t>
   </si>
   <si>
+    <t>altParcelId</t>
+  </si>
+  <si>
+    <t>backupParcelId2</t>
+  </si>
+  <si>
+    <t>id = ParcelId("01-2N-10-0000-001F-0100", "FL")</t>
+  </si>
+  <si>
+    <t>parse_raw_parcel_summary(second_column_contents)</t>
+  </si>
+  <si>
+    <t>construct_beacon_schneidercorp_url(rawParcelId)</t>
+  </si>
+  <si>
+    <t>ParcelId(parcelId).searchString</t>
+  </si>
+  <si>
+    <t>parcelnumb</t>
+  </si>
+  <si>
+    <t>original_address</t>
+  </si>
+  <si>
+    <t>legaldesc</t>
+  </si>
+  <si>
+    <t>{usecode+”00”, lbcs_activity, lbcs_function, lbcs_site, lbcs_ownership}</t>
+  </si>
+  <si>
+    <t>ll_gisacre</t>
+  </si>
+  <si>
+    <t>homestead_exemption</t>
+  </si>
+  <si>
+    <t>ogc_fid or ll_uuid (or unstable human readable field “path”)</t>
+  </si>
+  <si>
+    <t>{[lat, lon],…, [lat, lon]}</t>
+  </si>
+  <si>
+    <t>parcelnumb_no_formatting</t>
+  </si>
+  <si>
     <t>altParcelId1</t>
   </si>
   <si>
-    <t>altParcelId2</t>
-  </si>
-  <si>
     <t>SalesTable</t>
   </si>
   <si>
@@ -185,6 +263,18 @@
     <t>grantor</t>
   </si>
   <si>
+    <t>saleprice</t>
+  </si>
+  <si>
+    <t>book + “/“ + page</t>
+  </si>
+  <si>
+    <t>improvqual</t>
+  </si>
+  <si>
+    <t>saledate</t>
+  </si>
+  <si>
     <t>SketchesTable</t>
   </si>
   <si>
@@ -197,6 +287,12 @@
     <t>Url</t>
   </si>
   <si>
+    <t>taxBillNumber</t>
+  </si>
+  <si>
+    <t>tax_id</t>
+  </si>
+  <si>
     <t>ValuationTable</t>
   </si>
   <si>
@@ -228,9 +324,6 @@
   </si>
   <si>
     <t>justvalhomestead</t>
-  </si>
-  <si>
-    <t>???</t>
   </si>
   <si>
     <t>lnd_val</t>
@@ -276,7 +369,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +397,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -427,7 +532,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -461,7 +566,46 @@
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -473,29 +617,20 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,6 +653,8 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffed220b"/>
+      <rgbColor rgb="fffff056"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="fffefffe"/>
     </indexedColors>
@@ -1556,7 +1693,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20.7891" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
     <col min="2" max="17" width="16.3516" style="1" customWidth="1"/>
     <col min="18" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -1681,46 +1818,110 @@
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
+      <c r="B5" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="N5" s="13">
+        <v>2</v>
+      </c>
+      <c r="O5" s="13">
+        <v>2</v>
+      </c>
+      <c r="P5" s="13">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s" s="12">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="O6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="Q6" t="s" s="15">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1739,7 +1940,7 @@
       <c r="Q7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1758,7 +1959,7 @@
       <c r="Q8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1777,7 +1978,7 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -1796,7 +1997,7 @@
       <c r="Q10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -1815,7 +2016,7 @@
       <c r="Q11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="11"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1834,7 +2035,7 @@
       <c r="Q12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="11"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1853,7 +2054,7 @@
       <c r="Q13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="11"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1872,7 +2073,7 @@
       <c r="Q14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="11"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1891,7 +2092,7 @@
       <c r="Q15" s="10"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="11"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1910,7 +2111,7 @@
       <c r="Q16" s="10"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="11"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1929,7 +2130,7 @@
       <c r="Q17" s="10"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="11"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1948,7 +2149,7 @@
       <c r="Q18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="11"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1967,7 +2168,7 @@
       <c r="Q19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="11"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1986,7 +2187,7 @@
       <c r="Q20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="11"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -2005,7 +2206,7 @@
       <c r="Q21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="11"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -2024,7 +2225,7 @@
       <c r="Q22" s="10"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="11"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -2043,7 +2244,7 @@
       <c r="Q23" s="10"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="11"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2062,7 +2263,7 @@
       <c r="Q24" s="10"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="11"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2081,7 +2282,7 @@
       <c r="Q25" s="10"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="11"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -2100,7 +2301,7 @@
       <c r="Q26" s="10"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="11"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -2143,13 +2344,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.1562" style="17" customWidth="1"/>
+    <col min="3" max="3" width="18.6641" style="17" customWidth="1"/>
+    <col min="4" max="4" width="21.2109" style="17" customWidth="1"/>
+    <col min="5" max="5" width="21.2656" style="17" customWidth="1"/>
+    <col min="6" max="6" width="22.1562" style="17" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2162,22 +2368,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>18</v>
       </c>
@@ -2201,24 +2407,44 @@
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s" s="15">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -2226,7 +2452,7 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2234,7 +2460,7 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2242,7 +2468,7 @@
       <c r="F9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2250,7 +2476,7 @@
       <c r="F10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2282,13 +2508,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="19" customWidth="1"/>
+    <col min="2" max="2" width="42.8906" style="19" customWidth="1"/>
+    <col min="3" max="7" width="16.3516" style="19" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2302,34 +2530,46 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>34</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" ht="44.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="B3" t="s" s="20">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s" s="21">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" ht="32.05" customHeight="1">
       <c r="A4" t="s" s="8">
@@ -2346,26 +2586,50 @@
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="B5" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s" s="12">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="11">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s" s="12">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s" s="12">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s" s="12">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -2374,7 +2638,7 @@
       <c r="G7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2383,7 +2647,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2392,7 +2656,7 @@
       <c r="G9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2401,7 +2665,7 @@
       <c r="G10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2434,13 +2698,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="11" width="16.3516" style="14" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="14" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="22" customWidth="1"/>
+    <col min="2" max="2" width="38.4297" style="22" customWidth="1"/>
+    <col min="3" max="7" width="16.3516" style="22" customWidth="1"/>
+    <col min="8" max="8" width="20.2422" style="22" customWidth="1"/>
+    <col min="9" max="9" width="22.9531" style="22" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="22" customWidth="1"/>
+    <col min="11" max="11" width="20.3594" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2458,50 +2728,70 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s" s="3">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="44.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="B3" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s" s="21">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s" s="23">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s" s="23">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" ht="32.05" customHeight="1">
       <c r="A4" t="s" s="8">
@@ -2522,34 +2812,74 @@
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
+      <c r="B5" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="K5" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" ht="68.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="11">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="12">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s" s="12">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s" s="12">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s" s="24">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s" s="12">
+        <v>68</v>
+      </c>
+      <c r="J6" t="s" s="12">
+        <v>69</v>
+      </c>
+      <c r="K6" t="s" s="12">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -2562,7 +2892,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2575,7 +2905,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2588,7 +2918,7 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2601,7 +2931,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2638,14 +2968,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="1.17188" style="15" customWidth="1"/>
-    <col min="2" max="11" width="16.3516" style="15" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="15" customWidth="1"/>
+    <col min="1" max="1" width="1.17188" style="25" customWidth="1"/>
+    <col min="2" max="11" width="16.3516" style="25" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="B1" t="s" s="2">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2662,34 +2992,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
       <c r="B3" t="s" s="5">
         <v>18</v>
       </c>
@@ -2721,32 +3051,68 @@
       <c r="B5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
+      <c r="C5" s="18">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="13">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s" s="12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
       <c r="B6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s" s="12">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s" s="12">
+        <v>84</v>
+      </c>
+      <c r="J6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s" s="12">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="B7" s="11"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -2758,7 +3124,7 @@
       <c r="K7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="B8" s="11"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -2770,7 +3136,7 @@
       <c r="K8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="B9" s="11"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -2782,7 +3148,7 @@
       <c r="K9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="B10" s="11"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2794,7 +3160,7 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -2830,13 +3196,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="16.3516" style="16" customWidth="1"/>
+    <col min="1" max="2" width="16.3516" style="26" customWidth="1"/>
+    <col min="3" max="16384" width="16.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -2845,10 +3211,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>18</v>
       </c>
@@ -2864,32 +3230,36 @@
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
+      <c r="B5" t="s" s="11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -2909,7 +3279,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B11"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2917,71 +3287,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="17" customWidth="1"/>
-    <col min="3" max="16384" width="16.3516" style="17" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="18">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+      <c r="B2" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s" s="28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>18</v>
       </c>
       <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" ht="32.05" customHeight="1">
       <c r="A4" t="s" s="8">
         <v>19</v>
       </c>
       <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
+      <c r="B5" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s" s="12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3004,17 +3395,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="19" customWidth="1"/>
-    <col min="3" max="3" width="18.3672" style="19" customWidth="1"/>
-    <col min="4" max="7" width="16.3516" style="19" customWidth="1"/>
-    <col min="8" max="8" width="17.6406" style="19" customWidth="1"/>
-    <col min="9" max="10" width="16.3516" style="19" customWidth="1"/>
-    <col min="11" max="16384" width="16.3516" style="19" customWidth="1"/>
+    <col min="1" max="2" width="16.3516" style="29" customWidth="1"/>
+    <col min="3" max="3" width="18.3672" style="29" customWidth="1"/>
+    <col min="4" max="7" width="16.3516" style="29" customWidth="1"/>
+    <col min="8" max="8" width="17.6406" style="29" customWidth="1"/>
+    <col min="9" max="10" width="16.3516" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="16.3516" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3031,34 +3422,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>18</v>
       </c>
@@ -3100,40 +3491,40 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
+    <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s" s="20">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s" s="21">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s" s="22">
-        <v>71</v>
-      </c>
-      <c r="E6" t="s" s="22">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s" s="22">
-        <v>73</v>
-      </c>
-      <c r="G6" t="s" s="22">
-        <v>74</v>
-      </c>
-      <c r="H6" t="s" s="21">
-        <v>75</v>
-      </c>
-      <c r="I6" t="s" s="22">
-        <v>76</v>
-      </c>
-      <c r="J6" t="s" s="21">
-        <v>70</v>
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="30">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="31">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s" s="31">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s" s="31">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s" s="31">
+        <v>105</v>
+      </c>
+      <c r="H6" t="s" s="32">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s" s="31">
+        <v>107</v>
+      </c>
+      <c r="J6" t="s" s="15">
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -3145,7 +3536,7 @@
       <c r="J7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="11"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -3157,7 +3548,7 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="11"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3169,7 +3560,7 @@
       <c r="J9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -3181,7 +3572,7 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="11"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>

</xml_diff>

<commit_message>
Fixed ValuationTable sheet to match commit #8cc21f9
</commit_message>
<xml_diff>
--- a/DatasetConfiguration/DatasetDocumentation.xlsx
+++ b/DatasetConfiguration/DatasetDocumentation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
   <si>
     <t>BuildingInfoTable</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>landAgriculturalValue</t>
+  </si>
+  <si>
+    <t>agriculturalMarketValue</t>
   </si>
   <si>
     <t>justMarketValue</t>
@@ -3387,7 +3390,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J11"/>
+  <dimension ref="A2:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -3397,10 +3400,12 @@
   <cols>
     <col min="1" max="2" width="16.3516" style="29" customWidth="1"/>
     <col min="3" max="3" width="18.3672" style="29" customWidth="1"/>
-    <col min="4" max="7" width="16.3516" style="29" customWidth="1"/>
-    <col min="8" max="8" width="17.6406" style="29" customWidth="1"/>
-    <col min="9" max="10" width="16.3516" style="29" customWidth="1"/>
-    <col min="11" max="16384" width="16.3516" style="29" customWidth="1"/>
+    <col min="4" max="5" width="16.3516" style="29" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="29" customWidth="1"/>
+    <col min="7" max="8" width="16.3516" style="29" customWidth="1"/>
+    <col min="9" max="9" width="17.6406" style="29" customWidth="1"/>
+    <col min="10" max="11" width="16.3516" style="29" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -3416,6 +3421,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" ht="32.25" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -3439,14 +3445,17 @@
       <c r="G2" t="s" s="4">
         <v>97</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" t="s" s="4">
         <v>98</v>
       </c>
-      <c r="I2" t="s" s="4">
+      <c r="I2" t="s" s="3">
         <v>99</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" t="s" s="4">
         <v>100</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="32.25" customHeight="1">
@@ -3462,6 +3471,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" ht="32.05" customHeight="1">
       <c r="A4" t="s" s="8">
@@ -3476,50 +3486,75 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
       <c r="A5" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="B5" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="H5" s="13">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="J5" s="13">
+        <v>3</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="8">
         <v>22</v>
       </c>
       <c r="B6" t="s" s="30">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s" s="15">
         <v>23</v>
       </c>
       <c r="D6" t="s" s="31">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s" s="31">
-        <v>103</v>
-      </c>
-      <c r="F6" t="s" s="31">
         <v>104</v>
+      </c>
+      <c r="F6" t="s" s="15">
+        <v>23</v>
       </c>
       <c r="G6" t="s" s="31">
         <v>105</v>
       </c>
-      <c r="H6" t="s" s="32">
+      <c r="H6" t="s" s="31">
         <v>106</v>
       </c>
-      <c r="I6" t="s" s="31">
+      <c r="I6" t="s" s="32">
         <v>107</v>
       </c>
-      <c r="J6" t="s" s="15">
+      <c r="J6" t="s" s="31">
+        <v>108</v>
+      </c>
+      <c r="K6" t="s" s="15">
         <v>23</v>
       </c>
     </row>
@@ -3534,6 +3569,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="16"/>
@@ -3546,6 +3582,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="16"/>
@@ -3558,6 +3595,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="16"/>
@@ -3570,6 +3608,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="16"/>
@@ -3582,10 +3621,11 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
FINAL: SQlite and DatasetDocumentation Sync
</commit_message>
<xml_diff>
--- a/DatasetConfiguration/DatasetDocumentation.xlsx
+++ b/DatasetConfiguration/DatasetDocumentation.xlsx
@@ -92,7 +92,8 @@
     <t>DATA NOT AVAILABLE</t>
   </si>
   <si>
-    <t>recrdareano</t>
+    <t>STANDARD: recrdareano
+PREMIUM: ll_bldg_footprint_sqft &amp;ll_bldg_count</t>
   </si>
   <si>
     <t>yearbuilt</t>
@@ -278,13 +279,13 @@
     <t>SketchesTable</t>
   </si>
   <si>
-    <t>pngFilename</t>
+    <t>pngFilenameSource</t>
   </si>
   <si>
     <t>TaxCollectorTable</t>
   </si>
   <si>
-    <t>Url</t>
+    <t>url</t>
   </si>
   <si>
     <t>taxBillNumber</t>
@@ -1697,7 +1698,9 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
-    <col min="2" max="17" width="16.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.9688" style="1" customWidth="1"/>
+    <col min="4" max="17" width="16.3516" style="1" customWidth="1"/>
     <col min="18" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3199,7 +3202,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="26" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="26" customWidth="1"/>
+    <col min="2" max="2" width="19.7188" style="26" customWidth="1"/>
     <col min="3" max="16384" width="16.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3237,7 +3241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="32.05" customHeight="1">
+    <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="8">
         <v>22</v>
       </c>

</xml_diff>